<commit_message>
Various updates during 2nd revision of Chapter 2 (Ern).
</commit_message>
<xml_diff>
--- a/Number_of_Inductions.xlsx
+++ b/Number_of_Inductions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92aa253a0c32209f/Documents/GitHub/Microbial_Interactions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{6B2A8FE3-2D00-48A4-9787-E8549A41ED7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AEE11CC-8297-4F25-BF7F-1C97ADBDCA4D}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{6B2A8FE3-2D00-48A4-9787-E8549A41ED7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDDE02D7-1462-4BCF-88C1-2A2817DDF85A}"/>
   <bookViews>
-    <workbookView xWindow="10776" yWindow="1368" windowWidth="12264" windowHeight="9192" xr2:uid="{364FD5EA-183C-4619-9EDA-458B5B11BC4E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{364FD5EA-183C-4619-9EDA-458B5B11BC4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>Relation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Type</t>
   </si>
@@ -48,19 +45,19 @@
     <t>Error</t>
   </si>
   <si>
-    <t>Talented</t>
-  </si>
-  <si>
     <t>fungus-fungus</t>
   </si>
   <si>
     <t>fungus-bacterium</t>
   </si>
   <si>
-    <t>bacterium-bacterium</t>
-  </si>
-  <si>
-    <t>Ecologically Relevant</t>
+    <t>Geographically distant</t>
+  </si>
+  <si>
+    <t>Geographically close</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -421,34 +418,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF47BE7-5557-462D-8542-9E31A1473D26}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>3.45</v>
@@ -459,10 +456,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>6.79</v>
@@ -473,43 +470,29 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>4.7300000000000004</v>
+        <v>2.17</v>
       </c>
       <c r="D4">
-        <v>0.54</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>2.17</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="D5">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="D6">
         <v>0.81</v>
       </c>
     </row>

</xml_diff>